<commit_message>
current vs max dV/dt graph
</commit_message>
<xml_diff>
--- a/analysis_scripts_iclamp/wk6.xlsx
+++ b/analysis_scripts_iclamp/wk6.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="87" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="240" uniqueCount="69">
   <si>
     <t>File Name</t>
   </si>
@@ -106,6 +106,120 @@
   </si>
   <si>
     <t>2024_09_18_03_0009.abf</t>
+  </si>
+  <si>
+    <t>2025_01_31_07_0005.abf</t>
+  </si>
+  <si>
+    <t>2024_11_15_03_0002.abf</t>
+  </si>
+  <si>
+    <t>Sweep_26</t>
+  </si>
+  <si>
+    <t>Sweep_27</t>
+  </si>
+  <si>
+    <t>Sweep_28</t>
+  </si>
+  <si>
+    <t>Sweep_29</t>
+  </si>
+  <si>
+    <t>Sweep_30</t>
+  </si>
+  <si>
+    <t>Sweep_31</t>
+  </si>
+  <si>
+    <t>Sweep_32</t>
+  </si>
+  <si>
+    <t>Sweep_33</t>
+  </si>
+  <si>
+    <t>Sweep_34</t>
+  </si>
+  <si>
+    <t>Sweep_35</t>
+  </si>
+  <si>
+    <t>Sweep_36</t>
+  </si>
+  <si>
+    <t>Sweep_37</t>
+  </si>
+  <si>
+    <t>Sweep_38</t>
+  </si>
+  <si>
+    <t>Sweep_39</t>
+  </si>
+  <si>
+    <t>Sweep_40</t>
+  </si>
+  <si>
+    <t>Sweep_41</t>
+  </si>
+  <si>
+    <t>Sweep_42</t>
+  </si>
+  <si>
+    <t>Sweep_43</t>
+  </si>
+  <si>
+    <t>Sweep_44</t>
+  </si>
+  <si>
+    <t>Sweep_45</t>
+  </si>
+  <si>
+    <t>Sweep_46</t>
+  </si>
+  <si>
+    <t>Sweep_47</t>
+  </si>
+  <si>
+    <t>Sweep_48</t>
+  </si>
+  <si>
+    <t>Sweep_49</t>
+  </si>
+  <si>
+    <t>Sweep_50</t>
+  </si>
+  <si>
+    <t>Sweep_51</t>
+  </si>
+  <si>
+    <t>Sweep_52</t>
+  </si>
+  <si>
+    <t>Sweep_53</t>
+  </si>
+  <si>
+    <t>Sweep_54</t>
+  </si>
+  <si>
+    <t>Sweep_55</t>
+  </si>
+  <si>
+    <t>Sweep_56</t>
+  </si>
+  <si>
+    <t>Sweep_57</t>
+  </si>
+  <si>
+    <t>Sweep_58</t>
+  </si>
+  <si>
+    <t>Sweep_59</t>
+  </si>
+  <si>
+    <t>Sweep_60</t>
+  </si>
+  <si>
+    <t>2023_07_06_04_0005.abf</t>
   </si>
 </sst>
 </file>
@@ -151,7 +265,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:BI4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -183,6 +297,41 @@
     <col min="24" max="24" width="10.140625" customWidth="true"/>
     <col min="25" max="25" width="10.140625" customWidth="true"/>
     <col min="26" max="26" width="10.140625" customWidth="true"/>
+    <col min="27" max="27" width="10.140625" customWidth="true"/>
+    <col min="28" max="28" width="10.140625" customWidth="true"/>
+    <col min="29" max="29" width="10.140625" customWidth="true"/>
+    <col min="30" max="30" width="10.140625" customWidth="true"/>
+    <col min="31" max="31" width="10.140625" customWidth="true"/>
+    <col min="32" max="32" width="10.140625" customWidth="true"/>
+    <col min="33" max="33" width="10.140625" customWidth="true"/>
+    <col min="34" max="34" width="10.140625" customWidth="true"/>
+    <col min="35" max="35" width="10.140625" customWidth="true"/>
+    <col min="36" max="36" width="10.140625" customWidth="true"/>
+    <col min="37" max="37" width="10.140625" customWidth="true"/>
+    <col min="38" max="38" width="10.140625" customWidth="true"/>
+    <col min="39" max="39" width="10.140625" customWidth="true"/>
+    <col min="40" max="40" width="10.140625" customWidth="true"/>
+    <col min="41" max="41" width="10.140625" customWidth="true"/>
+    <col min="42" max="42" width="10.140625" customWidth="true"/>
+    <col min="43" max="43" width="10.140625" customWidth="true"/>
+    <col min="44" max="44" width="10.140625" customWidth="true"/>
+    <col min="45" max="45" width="10.140625" customWidth="true"/>
+    <col min="46" max="46" width="10.140625" customWidth="true"/>
+    <col min="47" max="47" width="10.140625" customWidth="true"/>
+    <col min="48" max="48" width="10.140625" customWidth="true"/>
+    <col min="49" max="49" width="10.140625" customWidth="true"/>
+    <col min="50" max="50" width="10.140625" customWidth="true"/>
+    <col min="51" max="51" width="10.140625" customWidth="true"/>
+    <col min="52" max="52" width="10.140625" customWidth="true"/>
+    <col min="53" max="53" width="10.140625" customWidth="true"/>
+    <col min="54" max="54" width="10.140625" customWidth="true"/>
+    <col min="55" max="55" width="10.140625" customWidth="true"/>
+    <col min="56" max="56" width="10.140625" customWidth="true"/>
+    <col min="57" max="57" width="10.140625" customWidth="true"/>
+    <col min="58" max="58" width="10.140625" customWidth="true"/>
+    <col min="59" max="59" width="10.140625" customWidth="true"/>
+    <col min="60" max="60" width="10.140625" customWidth="true"/>
+    <col min="61" max="61" width="10.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -264,90 +413,300 @@
       <c r="Z1" s="0" t="s">
         <v>28</v>
       </c>
+      <c r="AA1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="BG1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="BH1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="BI1" s="0" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0">
+        <v>0</v>
+      </c>
+      <c r="L2" s="0">
         <v>1</v>
       </c>
-      <c r="D2" s="0">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0">
-        <v>1</v>
-      </c>
-      <c r="G2" s="0">
+      <c r="M2" s="0">
+        <v>3</v>
+      </c>
+      <c r="N2" s="0">
+        <v>5</v>
+      </c>
+      <c r="O2" s="0">
+        <v>6</v>
+      </c>
+      <c r="P2" s="0">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="0">
+        <v>8</v>
+      </c>
+      <c r="R2" s="0">
         <v>10</v>
       </c>
-      <c r="H2" s="0">
+      <c r="S2" s="0">
+        <v>10</v>
+      </c>
+      <c r="T2" s="0">
+        <v>11</v>
+      </c>
+      <c r="U2" s="0">
+        <v>12</v>
+      </c>
+      <c r="V2" s="0">
+        <v>13</v>
+      </c>
+      <c r="W2" s="0">
         <v>14</v>
       </c>
-      <c r="I2" s="0">
-        <v>17</v>
-      </c>
-      <c r="J2" s="0">
-        <v>20</v>
-      </c>
-      <c r="K2" s="0">
-        <v>22</v>
-      </c>
-      <c r="L2" s="0">
-        <v>23</v>
-      </c>
-      <c r="M2" s="0">
-        <v>25</v>
-      </c>
-      <c r="N2" s="0">
-        <v>26</v>
-      </c>
-      <c r="O2" s="0">
-        <v>27</v>
-      </c>
-      <c r="P2" s="0">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="0">
-        <v>29</v>
-      </c>
-      <c r="R2" s="0">
-        <v>30</v>
-      </c>
-      <c r="S2" s="0">
-        <v>30</v>
-      </c>
-      <c r="T2" s="0">
-        <v>31</v>
-      </c>
-      <c r="U2" s="0">
-        <v>32</v>
-      </c>
-      <c r="V2" s="0">
-        <v>32</v>
-      </c>
-      <c r="W2" s="0">
-        <v>33</v>
-      </c>
       <c r="X2" s="0">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="Y2" s="0">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="Z2" s="0">
-        <v>33</v>
+        <v>16</v>
+      </c>
+      <c r="AA2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="0">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0">
         <v>0</v>
@@ -362,67 +721,172 @@
         <v>0</v>
       </c>
       <c r="F3" s="0">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0">
         <v>1</v>
       </c>
-      <c r="G3" s="0">
+      <c r="M3" s="0">
+        <v>3</v>
+      </c>
+      <c r="N3" s="0">
+        <v>5</v>
+      </c>
+      <c r="O3" s="0">
+        <v>6</v>
+      </c>
+      <c r="P3" s="0">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="0">
+        <v>8</v>
+      </c>
+      <c r="R3" s="0">
         <v>10</v>
       </c>
-      <c r="H3" s="0">
+      <c r="S3" s="0">
+        <v>10</v>
+      </c>
+      <c r="T3" s="0">
+        <v>11</v>
+      </c>
+      <c r="U3" s="0">
+        <v>12</v>
+      </c>
+      <c r="V3" s="0">
         <v>13</v>
       </c>
-      <c r="I3" s="0">
-        <v>17</v>
-      </c>
-      <c r="J3" s="0">
-        <v>20</v>
-      </c>
-      <c r="K3" s="0">
-        <v>22</v>
-      </c>
-      <c r="L3" s="0">
-        <v>23</v>
-      </c>
-      <c r="M3" s="0">
-        <v>25</v>
-      </c>
-      <c r="N3" s="0">
-        <v>27</v>
-      </c>
-      <c r="O3" s="0">
-        <v>28</v>
-      </c>
-      <c r="P3" s="0">
-        <v>28</v>
-      </c>
-      <c r="Q3" s="0">
-        <v>29</v>
-      </c>
-      <c r="R3" s="0">
-        <v>30</v>
-      </c>
-      <c r="S3" s="0">
-        <v>31</v>
-      </c>
-      <c r="T3" s="0">
-        <v>31</v>
-      </c>
-      <c r="U3" s="0">
-        <v>32</v>
-      </c>
-      <c r="V3" s="0">
-        <v>32</v>
-      </c>
       <c r="W3" s="0">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="X3" s="0">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="Y3" s="0">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="Z3" s="0">
-        <v>33</v>
+        <v>16</v>
+      </c>
+      <c r="AA3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BF3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="0">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>